<commit_message>
Folder with codes to revisit added, workload updated
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Day/Type</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>Some cells or styles in this workbook contain formatting that is not supported by the selected file format. These formats will be converted to the closest format available.</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -188,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,7 +205,39 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -209,38 +247,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -536,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -563,21 +574,43 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>40943</v>
-      </c>
-      <c r="B2" s="5" t="s">
+        <v>41309</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>40944</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
+        <v>41310</v>
+      </c>
+      <c r="B3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2">
+        <v>41311</v>
+      </c>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2">
+        <v>41312</v>
+      </c>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -628,78 +661,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="9"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
     </row>
     <row r="2" spans="2:5">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
     </row>
     <row r="3" spans="2:5">
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" spans="2:5" ht="45">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
     </row>
     <row r="5" spans="2:5">
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="2:5">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="16" t="s">
+      <c r="C6" s="5"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:5" ht="15.75" thickBot="1">
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="2:5" ht="45.75" thickBot="1">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="18">
+      <c r="C8" s="9"/>
+      <c r="D8" s="13"/>
+      <c r="E8" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:5">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" spans="2:5">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Worked on mergesort today and added more error handling in my own itoa
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Day/Type</t>
   </si>
@@ -56,6 +56,15 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>Algo</t>
+  </si>
+  <si>
+    <t>Quicksort</t>
+  </si>
+  <si>
+    <t>Mergesort</t>
   </si>
 </sst>
 </file>
@@ -93,7 +102,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -190,11 +199,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +258,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -245,12 +274,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -547,18 +570,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="5" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -571,46 +594,69 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>41309</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17"/>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>41310</v>
       </c>
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="16" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="2">
         <v>41311</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="2">
         <v>41312</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="2">
+        <v>41313</v>
+      </c>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Worked on Fibonacci today
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Day/Type</t>
   </si>
@@ -65,6 +65,15 @@
   </si>
   <si>
     <t>Mergesort</t>
+  </si>
+  <si>
+    <t>1.5H</t>
+  </si>
+  <si>
+    <t>0.5h</t>
+  </si>
+  <si>
+    <t>Fibonacci</t>
   </si>
 </sst>
 </file>
@@ -214,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -275,6 +284,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,7 +585,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -646,9 +658,18 @@
       <c r="A5" s="2">
         <v>41312</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
+      <c r="B5" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">

</xml_diff>

<commit_message>
Updated hours for the week end, wrote a function to check prime numbers and made ITOA functions a bit safer and throw exceptions
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Day/Type</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Some cells or styles in this workbook contain formatting that is not supported by the selected file format. These formats will be converted to the closest format available.</t>
   </si>
   <si>
-    <t>2h</t>
-  </si>
-  <si>
     <t>1h</t>
   </si>
   <si>
@@ -74,6 +71,30 @@
   </si>
   <si>
     <t>Fibonacci</t>
+  </si>
+  <si>
+    <t>1H</t>
+  </si>
+  <si>
+    <t>0H</t>
+  </si>
+  <si>
+    <t>0.5H</t>
+  </si>
+  <si>
+    <t>isPrime</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>3H</t>
   </si>
 </sst>
 </file>
@@ -111,7 +132,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -139,30 +160,6 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -212,11 +209,20 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -246,10 +252,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -261,10 +267,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -273,20 +279,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,35 +610,36 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>13</v>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2">
         <v>41309</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
         <v>41310</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
+      <c r="E3" s="17" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -642,16 +647,16 @@
         <v>41311</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
+      <c r="E4" s="17" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -659,29 +664,83 @@
         <v>41312</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="E5" s="18" t="s">
         <v>17</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="21" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2">
         <v>41313</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
+      <c r="B6" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="2">
+        <v>41314</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="2">
+        <v>41315</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="2">
+        <v>41316</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="16" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B2:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
wrote a smart pointer class and reference counting class + changed ITOA for use of smart pointer and exceptions handling
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Day/Type</t>
   </si>
@@ -95,6 +95,15 @@
   </si>
   <si>
     <t>3h</t>
+  </si>
+  <si>
+    <t>0h</t>
+  </si>
+  <si>
+    <t>2h</t>
+  </si>
+  <si>
+    <t>2.5H</t>
   </si>
 </sst>
 </file>
@@ -586,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -732,7 +741,7 @@
         <v>41316</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>18</v>
@@ -741,6 +750,51 @@
         <v>18</v>
       </c>
       <c r="E9" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2">
+        <v>41317</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2">
+        <v>41318</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2">
+        <v>41319</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Worked on Bubble sort today
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="30">
   <si>
     <t>Day/Type</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>2.5H</t>
+  </si>
+  <si>
+    <t>BubbleSort</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -287,10 +290,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,7 +597,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -627,12 +626,12 @@
       <c r="A2" s="2">
         <v>41309</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2">
@@ -647,7 +646,7 @@
       <c r="D3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="16" t="s">
         <v>12</v>
       </c>
     </row>
@@ -664,7 +663,7 @@
       <c r="D4" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
     </row>
@@ -681,7 +680,7 @@
       <c r="D5" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>16</v>
       </c>
     </row>
@@ -698,7 +697,7 @@
       <c r="D6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="17" t="s">
         <v>21</v>
       </c>
     </row>
@@ -715,7 +714,7 @@
       <c r="D7" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>20</v>
       </c>
     </row>
@@ -792,10 +791,12 @@
         <v>41319</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="C12" s="15" t="s">
+        <v>19</v>
+      </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on reversing words, in a string
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Day/Type</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>0.75H</t>
+  </si>
+  <si>
+    <t>Reverse words</t>
   </si>
 </sst>
 </file>
@@ -597,10 +603,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -804,6 +810,23 @@
       </c>
       <c r="E12" s="16" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2">
+        <v>41320</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked on a function that finds the next palindromic number, it not itself
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
   <si>
     <t>Day/Type</t>
   </si>
@@ -116,6 +116,9 @@
   </si>
   <si>
     <t>Reverse words</t>
+  </si>
+  <si>
+    <t>Next Palindrome</t>
   </si>
 </sst>
 </file>
@@ -603,15 +606,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="5" width="14.28515625" customWidth="1"/>
+    <col min="1" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -827,6 +831,23 @@
       </c>
       <c r="E13" s="16" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2">
+        <v>41321</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on finding the greatest common divisor, through iteration and recursion
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
   <si>
     <t>Day/Type</t>
   </si>
@@ -119,6 +119,9 @@
   </si>
   <si>
     <t>Next Palindrome</t>
+  </si>
+  <si>
+    <t>Greatest Common Divisor</t>
   </si>
 </sst>
 </file>
@@ -606,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -844,10 +847,27 @@
         <v>17</v>
       </c>
       <c r="D14" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="16" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2">
+        <v>41322</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Odd Even Sort
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
   <si>
     <t>Day/Type</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>ShellSort</t>
+  </si>
+  <si>
+    <t>Odd-Even Sort</t>
   </si>
 </sst>
 </file>
@@ -612,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -905,6 +908,23 @@
       </c>
       <c r="E17" s="16" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2">
+        <v>41325</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="16" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on math problems, changed decimal to fractions function and find angle between two hands of a clock
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="38">
   <si>
     <t>Day/Type</t>
   </si>
@@ -128,6 +128,9 @@
   </si>
   <si>
     <t>Odd-Even Sort</t>
+  </si>
+  <si>
+    <t>Decimal to Fraction</t>
   </si>
 </sst>
 </file>
@@ -615,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -925,6 +928,23 @@
       </c>
       <c r="E18" s="16" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="2">
+        <v>41326</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
angles between two hands more accurate, work on recursive swapping
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
   <si>
     <t>Day/Type</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t>Cocktail Shake Sort</t>
+  </si>
+  <si>
+    <t>Away</t>
   </si>
 </sst>
 </file>
@@ -171,7 +174,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -264,11 +267,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -326,6 +353,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -621,10 +657,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -952,7 +988,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2">
-        <v>41326</v>
+        <v>41327</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>18</v>
@@ -967,9 +1003,38 @@
         <v>38</v>
       </c>
     </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="2">
+        <v>41328</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2">
+        <v>41329</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Commiting workload, mostly just readings
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="42">
   <si>
     <t>Day/Type</t>
   </si>
@@ -663,10 +663,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1506,8 +1506,225 @@
         <v>22</v>
       </c>
     </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2">
+        <v>41359</v>
+      </c>
+      <c r="B52" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C52" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2">
+        <v>41360</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D53" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2">
+        <v>41361</v>
+      </c>
+      <c r="B54" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2">
+        <v>41362</v>
+      </c>
+      <c r="B55" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C55" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2">
+        <v>41363</v>
+      </c>
+      <c r="B56" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="20"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2">
+        <v>41364</v>
+      </c>
+      <c r="B57" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="19"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="20"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2">
+        <v>41365</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="20"/>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2">
+        <v>41366</v>
+      </c>
+      <c r="B59" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C59" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2">
+        <v>41367</v>
+      </c>
+      <c r="B60" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C60" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2">
+        <v>41368</v>
+      </c>
+      <c r="B61" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C61" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2">
+        <v>41369</v>
+      </c>
+      <c r="B62" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2">
+        <v>41370</v>
+      </c>
+      <c r="B63" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C63" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2">
+        <v>41371</v>
+      </c>
+      <c r="B64" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C64" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2">
+        <v>41372</v>
+      </c>
+      <c r="B65" s="15"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+      <c r="E65" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:E57"/>
+    <mergeCell ref="B58:E58"/>
     <mergeCell ref="B42:E42"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B22:E22"/>

</xml_diff>

<commit_message>
commit workload, no more commit for a little while, i need to move
</commit_message>
<xml_diff>
--- a/workload.xlsx
+++ b/workload.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="45">
   <si>
     <t>Day/Type</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>Selection Sort</t>
+  </si>
+  <si>
+    <t>BRISBANE TRIP TO THE STUDIOS</t>
   </si>
 </sst>
 </file>
@@ -669,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E71"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1834,8 +1837,71 @@
         <v>22</v>
       </c>
     </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2">
+        <v>41379</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C72" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2">
+        <v>41380</v>
+      </c>
+      <c r="B73" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C73" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2">
+        <v>41381</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C74" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2">
+        <v>41382</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C75" s="19"/>
+      <c r="D75" s="19"/>
+      <c r="E75" s="20"/>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
+    <mergeCell ref="B75:E75"/>
     <mergeCell ref="B56:E56"/>
     <mergeCell ref="B57:E57"/>
     <mergeCell ref="B58:E58"/>

</xml_diff>